<commit_message>
Signed-off-by: Daragh K. Carroll <Daragh.K.Carroll@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/DCarroll Assignment 1.xlsx
+++ b/DCarroll Assignment 1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00201097\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00201097\Desktop\Computer-Graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670"/>
+    <workbookView xWindow="600" yWindow="120" windowWidth="14115" windowHeight="8670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="102">
   <si>
     <t>z = -1</t>
   </si>
@@ -314,6 +314,30 @@
   </si>
   <si>
     <t>"(14.2, 4.5, 6.1)"</t>
+  </si>
+  <si>
+    <t>"(-275.4, -187.3, -93.6)"</t>
+  </si>
+  <si>
+    <t>"(45.2, 163.2, -197.8)"</t>
+  </si>
+  <si>
+    <t>"(110.3, 39.3, 163.4)"</t>
+  </si>
+  <si>
+    <t>"(-210.4, -311.2, 267.6)"</t>
+  </si>
+  <si>
+    <t>"(-99.3, -105.4, 281.4)"</t>
+  </si>
+  <si>
+    <t>"(221.3, 245.1, 177.2)"</t>
+  </si>
+  <si>
+    <t>"(286.4, 121.3, 538.4)"</t>
+  </si>
+  <si>
+    <t>"(-34.3, -229.2, 642.6)"</t>
   </si>
 </sst>
 </file>
@@ -642,22 +666,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,32 +714,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,13 +849,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
+      <xdr:colOff>446943</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>685547</xdr:colOff>
+      <xdr:colOff>560989</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>7327</xdr:rowOff>
     </xdr:to>
@@ -857,7 +881,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2395905" y="8191500"/>
+          <a:off x="2271347" y="8191500"/>
           <a:ext cx="2619854" cy="703385"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1079,6 +1103,116 @@
         <a:xfrm>
           <a:off x="7964368" y="9217269"/>
           <a:ext cx="2036885" cy="1445295"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>14654</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1254920</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>1018442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1846385" y="10997712"/>
+          <a:ext cx="3738747" cy="1003788"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>417639</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762004</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>1519353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2242043" y="12741519"/>
+          <a:ext cx="2850173" cy="1519353"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1389,7 +1523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1402,24 +1536,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1583,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1608,10 +1742,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="33"/>
+      <c r="E2" s="35"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1622,10 +1756,10 @@
     </row>
     <row r="3" spans="3:13" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="31"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="6"/>
       <c r="G3" s="11"/>
       <c r="H3" s="7"/>
@@ -1645,10 +1779,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1657,10 +1791,10 @@
     </row>
     <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E6" s="31"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1680,10 +1814,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="33"/>
+      <c r="E8" s="35"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1693,8 +1827,8 @@
     </row>
     <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1714,28 +1848,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="33"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="43"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="44"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1755,10 +1889,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="33"/>
+      <c r="E14" s="35"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1770,8 +1904,8 @@
     </row>
     <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="44"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1795,10 +1929,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="33"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1810,8 +1944,8 @@
     </row>
     <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1832,18 +1966,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="36" t="s">
+      <c r="E20" s="35"/>
+      <c r="F20" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="37"/>
-      <c r="H20" s="34" t="s">
+      <c r="G20" s="41"/>
+      <c r="H20" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="35"/>
+      <c r="I20" s="43"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1851,12 +1985,12 @@
     </row>
     <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="39"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="44"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1874,33 +2008,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="33"/>
+      <c r="E23" s="35"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="34" t="s">
+      <c r="L23" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="M23" s="35"/>
+      <c r="M23" s="43"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="44"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1913,10 +2047,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="35"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1927,8 +2061,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1946,15 +2080,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="43"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="32" t="s">
+      <c r="D29" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="33"/>
+      <c r="E29" s="35"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1965,11 +2099,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="38"/>
+      <c r="A30" s="38"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1987,44 +2121,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="33"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="36" t="s">
+      <c r="E32" s="35"/>
+      <c r="F32" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="32" t="s">
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="33"/>
+      <c r="M32" s="35"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="40"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="31"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="41"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="37"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -2036,47 +2170,32 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="35"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="31"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
@@ -2091,12 +2210,27 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2107,10 +2241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X57"/>
+  <dimension ref="A1:AB66"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L50" sqref="J50:L57"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59:M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2119,26 +2253,26 @@
     <col min="16" max="16" width="35.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42" t="s">
+    <row r="1" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42" t="s">
+      <c r="G2" s="28"/>
+      <c r="H2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="29" t="s">
         <v>40</v>
       </c>
       <c r="O2" t="s">
@@ -2150,36 +2284,46 @@
       <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="41"/>
-      <c r="U2" s="42" t="s">
+      <c r="T2" s="28"/>
+      <c r="U2" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="42" t="s">
+      <c r="V2" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="42" t="s">
+      <c r="W2" s="29" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44" t="s">
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="31">
         <v>0.94218150000000001</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44" t="s">
+      <c r="D3" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="44">
+      <c r="I3" s="31">
         <v>15</v>
       </c>
-      <c r="J3" s="44" t="s">
+      <c r="J3" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N3" t="s">
@@ -2194,38 +2338,50 @@
       <c r="Q3" t="s">
         <v>61</v>
       </c>
-      <c r="T3" s="43" t="s">
+      <c r="T3" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="44" t="s">
+      <c r="U3" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="44" t="s">
+      <c r="V3" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="W3" s="44" t="s">
+      <c r="W3" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="44" t="s">
+      <c r="Y3" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z3" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA3" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB3" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30"/>
+      <c r="B4" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="31">
         <v>-0.13378370000000001</v>
       </c>
-      <c r="D4" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44" t="s">
+      <c r="D4" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="44">
-        <v>0</v>
-      </c>
-      <c r="J4" s="44" t="s">
+      <c r="I4" s="31">
+        <v>0</v>
+      </c>
+      <c r="J4" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N4" t="s">
@@ -2240,38 +2396,50 @@
       <c r="Q4" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="43" t="s">
+      <c r="T4" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="44" t="s">
+      <c r="U4" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="V4" s="44" t="s">
+      <c r="V4" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="W4" s="44" t="s">
+      <c r="W4" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="44" t="s">
+      <c r="Y4" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z4" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA4" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB4" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="31">
         <v>0.30723919999999999</v>
       </c>
-      <c r="D5" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44" t="s">
+      <c r="D5" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="44">
-        <v>0</v>
-      </c>
-      <c r="J5" s="44" t="s">
+      <c r="I5" s="31">
+        <v>0</v>
+      </c>
+      <c r="J5" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N5" t="s">
@@ -2286,38 +2454,50 @@
       <c r="Q5" t="s">
         <v>61</v>
       </c>
-      <c r="T5" s="43" t="s">
+      <c r="T5" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="44" t="s">
+      <c r="U5" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="V5" s="44" t="s">
+      <c r="V5" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="W5" s="44" t="s">
+      <c r="W5" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44" t="s">
+      <c r="Y5" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z5" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA5" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB5" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="44">
-        <v>0</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44" t="s">
+      <c r="C6" s="31">
+        <v>0</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="44">
-        <v>0</v>
-      </c>
-      <c r="J6" s="44" t="s">
+      <c r="I6" s="31">
+        <v>0</v>
+      </c>
+      <c r="J6" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N6" t="s">
@@ -2332,38 +2512,50 @@
       <c r="Q6" t="s">
         <v>61</v>
       </c>
-      <c r="T6" s="43" t="s">
+      <c r="T6" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U6" s="44" t="s">
+      <c r="U6" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="V6" s="44" t="s">
+      <c r="V6" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="W6" s="44" t="s">
+      <c r="W6" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44" t="s">
+      <c r="Y6" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z6" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA6" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB6" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="31">
         <v>0.30723919999999999</v>
       </c>
-      <c r="D7" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="44" t="s">
+      <c r="D7" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="I7" s="44">
-        <v>0</v>
-      </c>
-      <c r="J7" s="44" t="s">
+      <c r="I7" s="31">
+        <v>0</v>
+      </c>
+      <c r="J7" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N7" t="s">
@@ -2378,38 +2570,50 @@
       <c r="Q7" t="s">
         <v>61</v>
       </c>
-      <c r="T7" s="43" t="s">
+      <c r="T7" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U7" s="44" t="s">
+      <c r="U7" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="V7" s="44" t="s">
+      <c r="V7" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="W7" s="44" t="s">
+      <c r="W7" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="44" t="s">
+      <c r="Y7" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z7" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA7" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB7" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="44">
+      <c r="C8" s="31">
         <v>0.71090759999999997</v>
       </c>
-      <c r="D8" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="44" t="s">
+      <c r="D8" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="44">
+      <c r="I8" s="31">
         <v>3</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="J8" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N8" t="s">
@@ -2424,38 +2628,50 @@
       <c r="Q8" t="s">
         <v>61</v>
       </c>
-      <c r="T8" s="43" t="s">
+      <c r="T8" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U8" s="44" t="s">
+      <c r="U8" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="V8" s="44" t="s">
+      <c r="V8" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="W8" s="44" t="s">
+      <c r="W8" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="44" t="s">
+      <c r="Y8" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z8" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA8" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB8" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="31">
         <v>-0.63262510000000005</v>
       </c>
-      <c r="D9" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="44" t="s">
+      <c r="D9" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="44">
-        <v>0</v>
-      </c>
-      <c r="J9" s="44" t="s">
+      <c r="I9" s="31">
+        <v>0</v>
+      </c>
+      <c r="J9" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N9" t="s">
@@ -2470,38 +2686,50 @@
       <c r="Q9" t="s">
         <v>61</v>
       </c>
-      <c r="T9" s="43" t="s">
+      <c r="T9" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="44" t="s">
+      <c r="U9" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="44" t="s">
+      <c r="V9" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="W9" s="44" t="s">
+      <c r="W9" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="44" t="s">
+      <c r="Y9" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z9" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA9" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB9" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="44">
-        <v>0</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="43"/>
-      <c r="H10" s="44" t="s">
+      <c r="C10" s="31">
+        <v>0</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="44">
-        <v>0</v>
-      </c>
-      <c r="J10" s="44" t="s">
+      <c r="I10" s="31">
+        <v>0</v>
+      </c>
+      <c r="J10" s="31" t="s">
         <v>42</v>
       </c>
       <c r="N10" t="s">
@@ -2516,396 +2744,408 @@
       <c r="Q10" t="s">
         <v>61</v>
       </c>
-      <c r="T10" s="43" t="s">
+      <c r="T10" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="44" t="s">
+      <c r="U10" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="V10" s="44" t="s">
+      <c r="V10" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="W10" s="44" t="s">
+      <c r="W10" s="31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43"/>
-      <c r="B11" s="44" t="s">
+      <c r="Y10" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z10" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA10" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB10" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="44">
+      <c r="C11" s="31">
         <v>-0.13378370000000001</v>
       </c>
-      <c r="D11" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="44" t="s">
+      <c r="D11" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="44">
-        <v>0</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="44" t="s">
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="44">
+      <c r="C12" s="31">
         <v>0.69044360000000005</v>
       </c>
-      <c r="D12" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="43"/>
-      <c r="H12" s="44" t="s">
+      <c r="D12" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="44">
-        <v>0</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="44" t="s">
+      <c r="I12" s="31">
+        <v>0</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="44">
+      <c r="C13" s="31">
         <v>0.71090759999999997</v>
       </c>
-      <c r="D13" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="43"/>
-      <c r="H13" s="44" t="s">
+      <c r="D13" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="44">
+      <c r="I13" s="31">
         <v>5</v>
       </c>
-      <c r="J13" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="44" t="s">
+      <c r="J13" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="44">
-        <v>0</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="44" t="s">
+      <c r="C14" s="31">
+        <v>0</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="44">
-        <v>0</v>
-      </c>
-      <c r="J14" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="P14" s="41"/>
-      <c r="Q14" s="42" t="s">
+      <c r="I14" s="31">
+        <v>0</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="42" t="s">
+      <c r="R14" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="S14" s="42" t="s">
+      <c r="S14" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="U14" s="41"/>
-      <c r="V14" s="42" t="s">
+      <c r="U14" s="28"/>
+      <c r="V14" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="W14" s="42" t="s">
+      <c r="W14" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="X14" s="42" t="s">
+      <c r="X14" s="29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43"/>
-      <c r="B15" s="44" t="s">
+    <row r="15" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="44">
-        <v>0</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" s="43"/>
-      <c r="H15" s="44" t="s">
+      <c r="C15" s="31">
+        <v>0</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="I15" s="44">
-        <v>0</v>
-      </c>
-      <c r="J15" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="P15" s="43"/>
-      <c r="Q15" s="44" t="s">
+      <c r="I15" s="31">
+        <v>0</v>
+      </c>
+      <c r="J15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="R15" s="44">
+      <c r="R15" s="31">
         <v>1</v>
       </c>
-      <c r="S15" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U15" s="43" t="s">
+      <c r="S15" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U15" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V15" s="44" t="s">
+      <c r="V15" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="W15" s="44" t="s">
+      <c r="W15" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="X15" s="44" t="s">
+      <c r="X15" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="43"/>
-      <c r="B16" s="44" t="s">
+    <row r="16" spans="1:28" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="44">
-        <v>0</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="44" t="s">
+      <c r="C16" s="31">
+        <v>0</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="44">
-        <v>0</v>
-      </c>
-      <c r="J16" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="P16" s="43"/>
-      <c r="Q16" s="44" t="s">
+      <c r="I16" s="31">
+        <v>0</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="R16" s="44">
-        <v>0</v>
-      </c>
-      <c r="S16" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U16" s="43" t="s">
+      <c r="R16" s="31">
+        <v>0</v>
+      </c>
+      <c r="S16" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U16" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V16" s="44" t="s">
+      <c r="V16" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="W16" s="44" t="s">
+      <c r="W16" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="X16" s="44" t="s">
+      <c r="X16" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43"/>
-      <c r="B17" s="44" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="44">
-        <v>0</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="43"/>
-      <c r="H17" s="44" t="s">
+      <c r="C17" s="31">
+        <v>0</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="I17" s="44">
-        <v>0</v>
-      </c>
-      <c r="J17" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="P17" s="43"/>
-      <c r="Q17" s="44" t="s">
+      <c r="I17" s="31">
+        <v>0</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="R17" s="44">
-        <v>0</v>
-      </c>
-      <c r="S17" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U17" s="43" t="s">
+      <c r="R17" s="31">
+        <v>0</v>
+      </c>
+      <c r="S17" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U17" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V17" s="44" t="s">
+      <c r="V17" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="W17" s="44" t="s">
+      <c r="W17" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="X17" s="44" t="s">
+      <c r="X17" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="43"/>
-      <c r="B18" s="44" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="31">
         <v>1</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="43"/>
-      <c r="H18" s="44" t="s">
+      <c r="D18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="I18" s="44">
+      <c r="I18" s="31">
         <v>1</v>
       </c>
-      <c r="J18" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="P18" s="43"/>
-      <c r="Q18" s="44" t="s">
+      <c r="J18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="R18" s="44">
+      <c r="R18" s="31">
         <v>2</v>
       </c>
-      <c r="S18" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U18" s="43" t="s">
+      <c r="S18" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U18" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V18" s="44" t="s">
+      <c r="V18" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="W18" s="44" t="s">
+      <c r="W18" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="X18" s="44" t="s">
+      <c r="X18" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P19" s="43"/>
-      <c r="Q19" s="44" t="s">
+      <c r="P19" s="30"/>
+      <c r="Q19" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="R19" s="44">
-        <v>0</v>
-      </c>
-      <c r="S19" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U19" s="43" t="s">
+      <c r="R19" s="31">
+        <v>0</v>
+      </c>
+      <c r="S19" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U19" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V19" s="44" t="s">
+      <c r="V19" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="W19" s="44" t="s">
+      <c r="W19" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="X19" s="44" t="s">
+      <c r="X19" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P20" s="43"/>
-      <c r="Q20" s="44" t="s">
+      <c r="P20" s="30"/>
+      <c r="Q20" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="R20" s="44">
+      <c r="R20" s="31">
         <v>1</v>
       </c>
-      <c r="S20" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U20" s="43" t="s">
+      <c r="S20" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U20" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V20" s="44" t="s">
+      <c r="V20" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="W20" s="44" t="s">
+      <c r="W20" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="X20" s="44" t="s">
+      <c r="X20" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P21" s="43"/>
-      <c r="Q21" s="44" t="s">
+      <c r="P21" s="30"/>
+      <c r="Q21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="R21" s="44">
-        <v>0</v>
-      </c>
-      <c r="S21" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U21" s="43" t="s">
+      <c r="R21" s="31">
+        <v>0</v>
+      </c>
+      <c r="S21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U21" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V21" s="44" t="s">
+      <c r="V21" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="W21" s="44" t="s">
+      <c r="W21" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="X21" s="44" t="s">
+      <c r="X21" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P22" s="43"/>
-      <c r="Q22" s="44" t="s">
+      <c r="P22" s="30"/>
+      <c r="Q22" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="R22" s="44">
+      <c r="R22" s="31">
         <v>4</v>
       </c>
-      <c r="S22" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U22" s="43" t="s">
+      <c r="S22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U22" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V22" s="44" t="s">
+      <c r="V22" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="W22" s="44" t="s">
+      <c r="W22" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="X22" s="44" t="s">
+      <c r="X22" s="31" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2916,28 +3156,28 @@
       <c r="K23" t="s">
         <v>60</v>
       </c>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="44" t="s">
+      <c r="P23" s="30"/>
+      <c r="Q23" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="R23" s="44">
-        <v>0</v>
-      </c>
-      <c r="S23" s="44" t="s">
+      <c r="R23" s="31">
+        <v>0</v>
+      </c>
+      <c r="S23" s="31" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>14.132720000000001</v>
+        <v>-11.583320000000001</v>
       </c>
       <c r="C24">
         <f>B28</f>
-        <v>0.92171749999999997</v>
+        <v>-12.399050000000001</v>
       </c>
       <c r="D24">
         <f>B32</f>
-        <v>-0.66891860000000003</v>
+        <v>1.0441309999999999</v>
       </c>
       <c r="E24">
         <f>B36</f>
@@ -2949,38 +3189,38 @@
       <c r="K24" t="s">
         <v>63</v>
       </c>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="44" t="s">
+      <c r="P24" s="30"/>
+      <c r="Q24" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="R24" s="44">
-        <v>0</v>
-      </c>
-      <c r="S24" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U24" s="41"/>
-      <c r="V24" s="42" t="s">
+      <c r="R24" s="31">
+        <v>0</v>
+      </c>
+      <c r="S24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U24" s="28"/>
+      <c r="V24" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="W24" s="42" t="s">
+      <c r="W24" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="X24" s="42" t="s">
+      <c r="X24" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>-2.0067560000000002</v>
+        <v>-5.5555969999999997</v>
       </c>
       <c r="C25">
         <f t="shared" ref="C25:C27" si="0">B29</f>
-        <v>2.1327229999999999</v>
+        <v>5.3656370000000004</v>
       </c>
       <c r="D25">
         <f t="shared" ref="D25:D27" si="1">B33</f>
-        <v>3.4522179999999998</v>
+        <v>2.0845319999999998</v>
       </c>
       <c r="E25">
         <f t="shared" ref="E25:E27" si="2">B37</f>
@@ -2992,40 +3232,40 @@
       <c r="K25" t="s">
         <v>65</v>
       </c>
-      <c r="P25" s="43"/>
-      <c r="Q25" s="44" t="s">
+      <c r="P25" s="30"/>
+      <c r="Q25" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="R25" s="44">
+      <c r="R25" s="31">
         <v>1</v>
       </c>
-      <c r="S25" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U25" s="43" t="s">
+      <c r="S25" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U25" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V25" s="44" t="s">
+      <c r="V25" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="W25" s="44" t="s">
+      <c r="W25" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="X25" s="44" t="s">
+      <c r="X25" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>4.6085880000000001</v>
+        <v>-12.7182</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>-1.897875</v>
+        <v>7.4189530000000001</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>3.554538</v>
+        <v>-52.992519999999999</v>
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
@@ -3037,40 +3277,40 @@
       <c r="K26" t="s">
         <v>67</v>
       </c>
-      <c r="P26" s="43"/>
-      <c r="Q26" s="44" t="s">
+      <c r="P26" s="30"/>
+      <c r="Q26" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="R26" s="44">
+      <c r="R26" s="31">
         <v>-4</v>
       </c>
-      <c r="S26" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U26" s="43" t="s">
+      <c r="S26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U26" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V26" s="44" t="s">
+      <c r="V26" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="W26" s="44" t="s">
+      <c r="W26" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="X26" s="44" t="s">
+      <c r="X26" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
@@ -3082,32 +3322,32 @@
       <c r="K27" t="s">
         <v>69</v>
       </c>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="44" t="s">
+      <c r="P27" s="30"/>
+      <c r="Q27" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="R27" s="44">
-        <v>0</v>
-      </c>
-      <c r="S27" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U27" s="43" t="s">
+      <c r="R27" s="31">
+        <v>0</v>
+      </c>
+      <c r="S27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U27" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V27" s="44" t="s">
+      <c r="V27" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="W27" s="44" t="s">
+      <c r="W27" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="X27" s="44" t="s">
+      <c r="X27" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>0.92171749999999997</v>
+        <v>-12.399050000000001</v>
       </c>
       <c r="J28" t="s">
         <v>70</v>
@@ -3115,32 +3355,32 @@
       <c r="K28" t="s">
         <v>71</v>
       </c>
-      <c r="P28" s="43"/>
-      <c r="Q28" s="44" t="s">
+      <c r="P28" s="30"/>
+      <c r="Q28" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="R28" s="44">
-        <v>0</v>
-      </c>
-      <c r="S28" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U28" s="43" t="s">
+      <c r="R28" s="31">
+        <v>0</v>
+      </c>
+      <c r="S28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U28" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V28" s="44" t="s">
+      <c r="V28" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="W28" s="44" t="s">
+      <c r="W28" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="X28" s="44" t="s">
+      <c r="X28" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2.1327229999999999</v>
+        <v>5.3656370000000004</v>
       </c>
       <c r="J29" t="s">
         <v>72</v>
@@ -3148,32 +3388,32 @@
       <c r="K29" t="s">
         <v>73</v>
       </c>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="44" t="s">
+      <c r="P29" s="30"/>
+      <c r="Q29" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="R29" s="44">
-        <v>0</v>
-      </c>
-      <c r="S29" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U29" s="43" t="s">
+      <c r="R29" s="31">
+        <v>0</v>
+      </c>
+      <c r="S29" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U29" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V29" s="44" t="s">
+      <c r="V29" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="W29" s="44" t="s">
+      <c r="W29" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="X29" s="44" t="s">
+      <c r="X29" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>-1.897875</v>
+        <v>7.4189530000000001</v>
       </c>
       <c r="J30" t="s">
         <v>74</v>
@@ -3181,49 +3421,49 @@
       <c r="K30" t="s">
         <v>75</v>
       </c>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="44" t="s">
+      <c r="P30" s="30"/>
+      <c r="Q30" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="R30" s="44">
+      <c r="R30" s="31">
         <v>1</v>
       </c>
-      <c r="S30" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="U30" s="43" t="s">
+      <c r="S30" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U30" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V30" s="44" t="s">
+      <c r="V30" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="W30" s="44" t="s">
+      <c r="W30" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="X30" s="44" t="s">
+      <c r="X30" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>4</v>
-      </c>
-      <c r="U31" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="U31" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V31" s="44" t="s">
+      <c r="V31" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="W31" s="44" t="s">
+      <c r="W31" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="X31" s="44" t="s">
+      <c r="X31" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>-0.66891860000000003</v>
+        <v>1.0441309999999999</v>
       </c>
       <c r="J32" t="s">
         <v>59</v>
@@ -3231,32 +3471,32 @@
       <c r="K32" t="s">
         <v>76</v>
       </c>
-      <c r="P32" s="41"/>
-      <c r="Q32" s="42" t="s">
+      <c r="P32" s="28"/>
+      <c r="Q32" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="R32" s="42" t="s">
+      <c r="R32" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="S32" s="42" t="s">
+      <c r="S32" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="U32" s="43" t="s">
+      <c r="U32" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="V32" s="44" t="s">
+      <c r="V32" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="W32" s="44" t="s">
+      <c r="W32" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="X32" s="44" t="s">
+      <c r="X32" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>3.4522179999999998</v>
+        <v>2.0845319999999998</v>
       </c>
       <c r="J33" t="s">
         <v>62</v>
@@ -3264,22 +3504,22 @@
       <c r="K33" t="s">
         <v>77</v>
       </c>
-      <c r="P33" s="43" t="s">
+      <c r="P33" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="Q33" s="44" t="s">
+      <c r="Q33" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="R33" s="44" t="s">
+      <c r="R33" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="S33" s="44" t="s">
+      <c r="S33" s="31" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>3.554538</v>
+        <v>-52.992519999999999</v>
       </c>
       <c r="J34" t="s">
         <v>64</v>
@@ -3287,20 +3527,30 @@
       <c r="K34" t="s">
         <v>78</v>
       </c>
-      <c r="P34" s="43"/>
-      <c r="Q34" s="44" t="s">
+      <c r="P34" s="30"/>
+      <c r="Q34" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="R34" s="44">
+      <c r="R34" s="31">
         <v>14.132720000000001</v>
       </c>
-      <c r="S34" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S34" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U34" s="28"/>
+      <c r="V34" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="W34" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="X34" s="29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>-4</v>
+        <v>0</v>
       </c>
       <c r="J35" t="s">
         <v>66</v>
@@ -3308,18 +3558,28 @@
       <c r="K35" t="s">
         <v>79</v>
       </c>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="44" t="s">
+      <c r="P35" s="30"/>
+      <c r="Q35" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="R35" s="44">
+      <c r="R35" s="31">
         <v>-2.0067560000000002</v>
       </c>
-      <c r="S35" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S35" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U35" s="30"/>
+      <c r="V35" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="W35" s="31">
+        <v>-11.583320000000001</v>
+      </c>
+      <c r="X35" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0</v>
       </c>
@@ -3329,18 +3589,28 @@
       <c r="K36" t="s">
         <v>80</v>
       </c>
-      <c r="P36" s="43"/>
-      <c r="Q36" s="44" t="s">
+      <c r="P36" s="30"/>
+      <c r="Q36" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="R36" s="44">
+      <c r="R36" s="31">
         <v>4.6085880000000001</v>
       </c>
-      <c r="S36" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S36" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U36" s="30"/>
+      <c r="V36" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="W36" s="31">
+        <v>-5.5555969999999997</v>
+      </c>
+      <c r="X36" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0</v>
       </c>
@@ -3350,18 +3620,28 @@
       <c r="K37" t="s">
         <v>81</v>
       </c>
-      <c r="P37" s="43"/>
-      <c r="Q37" s="44" t="s">
+      <c r="P37" s="30"/>
+      <c r="Q37" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="R37" s="44">
+      <c r="R37" s="31">
         <v>2</v>
       </c>
-      <c r="S37" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S37" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U37" s="30"/>
+      <c r="V37" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="W37" s="31">
+        <v>-12.7182</v>
+      </c>
+      <c r="X37" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0</v>
       </c>
@@ -3371,18 +3651,28 @@
       <c r="K38" t="s">
         <v>82</v>
       </c>
-      <c r="P38" s="43"/>
-      <c r="Q38" s="44" t="s">
+      <c r="P38" s="30"/>
+      <c r="Q38" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="R38" s="44">
+      <c r="R38" s="31">
         <v>0.92171749999999997</v>
       </c>
-      <c r="S38" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S38" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U38" s="30"/>
+      <c r="V38" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="W38" s="31">
+        <v>0</v>
+      </c>
+      <c r="X38" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>1</v>
       </c>
@@ -3392,194 +3682,314 @@
       <c r="K39" t="s">
         <v>83</v>
       </c>
-      <c r="P39" s="43"/>
-      <c r="Q39" s="44" t="s">
+      <c r="P39" s="30"/>
+      <c r="Q39" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="R39" s="44">
+      <c r="R39" s="31">
         <v>2.1327229999999999</v>
       </c>
-      <c r="S39" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="40" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P40" s="43"/>
-      <c r="Q40" s="44" t="s">
+      <c r="S39" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U39" s="30"/>
+      <c r="V39" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="W39" s="31">
+        <v>-12.399050000000001</v>
+      </c>
+      <c r="X39" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P40" s="30"/>
+      <c r="Q40" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="R40" s="44">
+      <c r="R40" s="31">
         <v>-1.897875</v>
       </c>
-      <c r="S40" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S40" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U40" s="30"/>
+      <c r="V40" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="W40" s="31">
+        <v>5.3656370000000004</v>
+      </c>
+      <c r="X40" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>59</v>
       </c>
       <c r="K41" t="s">
         <v>84</v>
       </c>
-      <c r="P41" s="43"/>
-      <c r="Q41" s="44" t="s">
+      <c r="P41" s="30"/>
+      <c r="Q41" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="R41" s="44">
+      <c r="R41" s="31">
         <v>4</v>
       </c>
-      <c r="S41" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S41" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U41" s="30"/>
+      <c r="V41" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="W41" s="31">
+        <v>7.4189530000000001</v>
+      </c>
+      <c r="X41" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>62</v>
       </c>
       <c r="K42" t="s">
         <v>85</v>
       </c>
-      <c r="P42" s="43"/>
-      <c r="Q42" s="44" t="s">
+      <c r="P42" s="30"/>
+      <c r="Q42" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="R42" s="44">
+      <c r="R42" s="31">
         <v>-0.66891860000000003</v>
       </c>
-      <c r="S42" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S42" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U42" s="30"/>
+      <c r="V42" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="W42" s="31">
+        <v>0</v>
+      </c>
+      <c r="X42" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
         <v>64</v>
       </c>
       <c r="K43" t="s">
         <v>86</v>
       </c>
-      <c r="P43" s="43"/>
-      <c r="Q43" s="44" t="s">
+      <c r="P43" s="30"/>
+      <c r="Q43" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="R43" s="44">
+      <c r="R43" s="31">
         <v>3.4522179999999998</v>
       </c>
-      <c r="S43" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="44" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S43" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U43" s="30"/>
+      <c r="V43" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="W43" s="31">
+        <v>1.0441309999999999</v>
+      </c>
+      <c r="X43" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
         <v>66</v>
       </c>
       <c r="K44" t="s">
         <v>87</v>
       </c>
-      <c r="P44" s="43"/>
-      <c r="Q44" s="44" t="s">
+      <c r="P44" s="30"/>
+      <c r="Q44" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="R44" s="44">
+      <c r="R44" s="31">
         <v>3.554538</v>
       </c>
-      <c r="S44" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S44" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U44" s="30"/>
+      <c r="V44" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="W44" s="31">
+        <v>2.0845319999999998</v>
+      </c>
+      <c r="X44" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J45" t="s">
         <v>68</v>
       </c>
       <c r="K45" t="s">
         <v>88</v>
       </c>
-      <c r="P45" s="43"/>
-      <c r="Q45" s="44" t="s">
+      <c r="P45" s="30"/>
+      <c r="Q45" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="R45" s="44">
+      <c r="R45" s="31">
         <v>-4</v>
       </c>
-      <c r="S45" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S45" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U45" s="30"/>
+      <c r="V45" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="W45" s="31">
+        <v>-52.992519999999999</v>
+      </c>
+      <c r="X45" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>70</v>
       </c>
       <c r="K46" t="s">
         <v>89</v>
       </c>
-      <c r="P46" s="43"/>
-      <c r="Q46" s="44" t="s">
+      <c r="P46" s="30"/>
+      <c r="Q46" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="R46" s="44">
-        <v>0</v>
-      </c>
-      <c r="S46" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R46" s="31">
+        <v>0</v>
+      </c>
+      <c r="S46" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U46" s="30"/>
+      <c r="V46" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="W46" s="31">
+        <v>0</v>
+      </c>
+      <c r="X46" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
         <v>72</v>
       </c>
       <c r="K47" t="s">
         <v>90</v>
       </c>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="44" t="s">
+      <c r="P47" s="30"/>
+      <c r="Q47" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="R47" s="44">
-        <v>0</v>
-      </c>
-      <c r="S47" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="2:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="R47" s="31">
+        <v>0</v>
+      </c>
+      <c r="S47" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U47" s="30"/>
+      <c r="V47" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="W47" s="31">
+        <v>0</v>
+      </c>
+      <c r="X47" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J48" t="s">
         <v>74</v>
       </c>
       <c r="K48" t="s">
         <v>91</v>
       </c>
-      <c r="P48" s="43"/>
-      <c r="Q48" s="44" t="s">
+      <c r="P48" s="30"/>
+      <c r="Q48" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="R48" s="44">
-        <v>0</v>
-      </c>
-      <c r="S48" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="49" spans="10:19" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="P49" s="43"/>
-      <c r="Q49" s="44" t="s">
+      <c r="R48" s="31">
+        <v>0</v>
+      </c>
+      <c r="S48" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U48" s="30"/>
+      <c r="V48" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="W48" s="31">
+        <v>0</v>
+      </c>
+      <c r="X48" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="10:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P49" s="30"/>
+      <c r="Q49" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="R49" s="44">
+      <c r="R49" s="31">
         <v>1</v>
       </c>
-      <c r="S49" s="44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="50" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="S49" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="U49" s="30"/>
+      <c r="V49" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="W49" s="31">
+        <v>0</v>
+      </c>
+      <c r="X49" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="10:24" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J50" t="s">
         <v>59</v>
       </c>
       <c r="K50" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="51" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U50" s="30"/>
+      <c r="V50" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="W50" s="31">
+        <v>1</v>
+      </c>
+      <c r="X50" s="31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J51" t="s">
         <v>62</v>
       </c>
@@ -3587,7 +3997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J52" t="s">
         <v>64</v>
       </c>
@@ -3595,7 +4005,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J53" t="s">
         <v>66</v>
       </c>
@@ -3603,7 +4013,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J54" t="s">
         <v>68</v>
       </c>
@@ -3611,7 +4021,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J55" t="s">
         <v>70</v>
       </c>
@@ -3619,7 +4029,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J56" t="s">
         <v>72</v>
       </c>
@@ -3627,12 +4037,76 @@
         <v>90</v>
       </c>
     </row>
-    <row r="57" spans="10:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J57" t="s">
         <v>74</v>
       </c>
       <c r="K57" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J59" t="s">
+        <v>59</v>
+      </c>
+      <c r="K59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J60" t="s">
+        <v>62</v>
+      </c>
+      <c r="K60" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J61" t="s">
+        <v>64</v>
+      </c>
+      <c r="K61" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J62" t="s">
+        <v>66</v>
+      </c>
+      <c r="K62" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J63" t="s">
+        <v>68</v>
+      </c>
+      <c r="K63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="10:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J64" t="s">
+        <v>70</v>
+      </c>
+      <c r="K64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J65" t="s">
+        <v>72</v>
+      </c>
+      <c r="K65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="10:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J66" t="s">
+        <v>74</v>
+      </c>
+      <c r="K66" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>